<commit_message>
update db according heroku postgresql
</commit_message>
<xml_diff>
--- a/excel/reports/form/form.xlsx
+++ b/excel/reports/form/form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28005" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>login</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>class</t>
+  </si>
+  <si>
+    <t>ЛогинПользователя</t>
+  </si>
+  <si>
+    <t>ПарольПользователя</t>
+  </si>
+  <si>
+    <t>Максим</t>
+  </si>
+  <si>
+    <t>Масимов</t>
+  </si>
+  <si>
+    <t>Максимович</t>
+  </si>
+  <si>
+    <t>9-5</t>
   </si>
 </sst>
 </file>
@@ -374,13 +392,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="26.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -402,7 +423,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>